<commit_message>
Updated the Bill of Materials
Need to check that these motors are good, for multiple rotations.
If using cyclodial drives, does it need that many bearings?
</commit_message>
<xml_diff>
--- a/hardware/Bill of Materias.xlsx
+++ b/hardware/Bill of Materias.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ark_bot\hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\ark_bot\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2538E7-813D-461E-ABE7-C6254F286BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99346FE1-B84A-4DDC-B972-795CB91E7C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{030F082E-5C24-4BB9-8500-0DF140B02703}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{030F082E-5C24-4BB9-8500-0DF140B02703}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>(Not confirmed yet still confirming)</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Esp32 servo driver</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
     <t>Cost of 1</t>
   </si>
   <si>
@@ -90,6 +87,102 @@
   </si>
   <si>
     <t>Alluminium Extrusion</t>
+  </si>
+  <si>
+    <t>Maybes?</t>
+  </si>
+  <si>
+    <t>Serial Bus servo driver board</t>
+  </si>
+  <si>
+    <t>https://www.waveshare.com/bus-servo-adapter-a.htm</t>
+  </si>
+  <si>
+    <t>Doc Link</t>
+  </si>
+  <si>
+    <t>https://thepihut.com/products/serial-bus-servo-20kg-cm</t>
+  </si>
+  <si>
+    <t>https://thepihut.com/products/serial-bus-servo-driver-board</t>
+  </si>
+  <si>
+    <t>Raspberry Pi</t>
+  </si>
+  <si>
+    <t>Where I got them from:</t>
+  </si>
+  <si>
+    <t>3P - 5264 Male Female Connector Straight Pin Curved Pin housing</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005001317326647.html</t>
+  </si>
+  <si>
+    <t>16-30AWG 5 Colors DIY Wire Silicone Tinned Copper Electronic Wire</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Need to check which ratings are good</t>
+  </si>
+  <si>
+    <t>Check which camera</t>
+  </si>
+  <si>
+    <t>Check which Rpi</t>
+  </si>
+  <si>
+    <t>https://thepihut.com/products/flex-cable-for-raspberry-pi-camera-or-display-1-meter</t>
+  </si>
+  <si>
+    <t>1m Rpi Camera Cable</t>
+  </si>
+  <si>
+    <t>https://thepihut.com/products/zero-camera-cable-joiner-for-raspberry-pi-22-pin-to-22-pin</t>
+  </si>
+  <si>
+    <t>Depends on the camera, might need adapter</t>
+  </si>
+  <si>
+    <t>Camera cable joiner for Rpi</t>
+  </si>
+  <si>
+    <t>Generic PLA Filament</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/Assortment-Stainless-Replacement-Machine-Fastener/dp/B0B3MGZ7T2/ref=sr_1_6?crid=9ARCU7Y28MLT&amp;dib=eyJ2IjoiMSJ9.C4FsLbrPOEs2fHxOGtZx-Yzy25y3h3M5nm3AJqVb8UtL-l5hOJfxSnOtUWey-BzyblwG_oNMk-fuUQVmlwPJtTILvfQP1GJlT-n5zV1bsjICJIG9QTYGIlRVJ5NcdjhPkjEXSBNdAZ5bCQgtHEstEkMyQJP7kh9dYx_3MnHkRD_Zbp2nHn-faxKTCNXUhXx04A9y27RMimfiw3mpRHMv561qt8nZDI-_r9BdiEzBBfv8hpjG_8QnQB1oni_3ql9bHUxEWQ_bjcDldWVL0HPq9iSZK0I7U8dGP-5JMMy4iD0.-_2bx2N9cl4Ar-yZdVNqwQuqJ9hWPbPGkrUGiixozVQ&amp;dib_tag=se&amp;keywords=m3%2Bhex%2Bscrews&amp;qid=1753791385&amp;sprefix=m3%2Bhex%2Bscrews%2Caps%2C82&amp;sr=8-6&amp;th=1</t>
+  </si>
+  <si>
+    <t>Colour doesn’t matter to me, 2 rolls to be safe</t>
+  </si>
+  <si>
+    <t>Generic M3 Bots and Nuts set</t>
+  </si>
+  <si>
+    <t>Total Cost:</t>
+  </si>
+  <si>
+    <t>20 pcs  688-2RS Bearing</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/dp/B0CH2WXRX9?ref_=ppx_hzsearch_conn_dt_b_fed_asin_title_4&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/HANGLIFE-Threaded-Inserts-Printing-Components/dp/B0CS6VZYL8/ref=sr_1_2_sspa?crid=2CO97LADPPFEZ&amp;dib=eyJ2IjoiMSJ9.lbVPV95BhrJYDjAUEXZD73UM97ZiMGi_1Nb7LF9OI13UMrlWH0Ak4Ta5Fb0GkGZt7t3Ax3jrqnl8mRNuMYaL43VtdnaBJut0XHf_unYSt-nmCgwpjhX6Bvutj6y6iMoHgmckI8SCuMZQXFSjfi6NTtRBUsb6yRBB7RxBzAn1j3xDK9AES_OkFUHSMxIsA-2HHiuZrSxobqvUGjL9Qj7NdQ6x2CJgd9SvtMhtf-mcKcJsOOC_68S7k_c7deVrn-v4H41M-43yP4bD_tB66u-yLqbudyqRl6MpRtCD2Qj2isY.gIt7QyFyezRyhfRmLZ-psPWW1VcSJtFEsy3-Bdh2ifY&amp;dib_tag=se&amp;keywords=m3%2Bthreaded%2Binserts&amp;qid=1753797012&amp;s=industrial&amp;sprefix=m3%2Bthreaded%2Binserts%2Cindustrial%2C84&amp;sr=1-2-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;th=1</t>
+  </si>
+  <si>
+    <t>100pcs M3 threaded inserts</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005007361806707.html?spm=a2g0o.productlist.main.4.7a265b85879DS0&amp;algo_pvid=13188671-718a-4056-bd7b-57393b720f00&amp;algo_exp_id=13188671-718a-4056-bd7b-57393b720f00-3&amp;pdp_ext_f=%7B%22order%22%3A%22267%22%2C%22eval%22%3A%221%22%7D&amp;pdp_npi=4%40dis%21GBP%214.03%214.03%21%21%2137.46%2137.46%21%40211b680e17537971187271601e7f00%2112000040429559553%21sea%21UK%216141414768%21X&amp;curPageLogUid=KQ3ssTxPUldf&amp;utparam-url=scene%3Asearch%7Cquery_from%3A</t>
+  </si>
+  <si>
+    <t>10 pcs 6706-2RS Bearing</t>
+  </si>
+  <si>
+    <t>Optional</t>
   </si>
 </sst>
 </file>
@@ -97,12 +190,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,14 +226,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -146,6 +260,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>93291</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>25669</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6020520-A601-5AB0-DE78-AC553DBFEC28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12961620" y="3850020"/>
+          <a:ext cx="6014031" cy="2942209"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -465,142 +628,353 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB0A156-46C5-43D5-BB16-CC69054DFD7A}">
-  <dimension ref="A2:I16"/>
+  <dimension ref="A2:U16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="40.21875" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="17" max="17" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
         <v>21.7</v>
       </c>
-      <c r="E3" s="1">
-        <f>D3*A3</f>
-        <v>151.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D4" s="1"/>
+      <c r="F3" s="1">
+        <f>E3*B3</f>
+        <v>173.6</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="1">
+        <f>SUM(F:F)</f>
+        <v>318.98</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>17</v>
+      </c>
+      <c r="U3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E16" si="0">D4*A4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F14" si="0">E4*B4</f>
+        <v>5</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="U4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1">
+        <v>60</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" t="s">
+        <v>48</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1">
+      <c r="S5" s="1">
         <v>17.3</v>
       </c>
-      <c r="E5" s="1">
+      <c r="U5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1">
+        <v>30</v>
+      </c>
+      <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>17.3</v>
-      </c>
-      <c r="I5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D6" s="1"/>
-      <c r="E6" s="1">
+        <v>30</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6" s="1">
+        <v>9.49</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="U6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E7" s="1"/>
-      <c r="I7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E8" s="1"/>
-      <c r="I8" t="s">
+      <c r="H7" s="4"/>
+      <c r="U7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E9" s="1"/>
-      <c r="I9" t="s">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.73</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.73</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E10" s="1"/>
-      <c r="I10" t="s">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="1">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="U9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="U10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="E11" s="1"/>
-      <c r="I11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E12" s="1"/>
-      <c r="I12" t="s">
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="U11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E13" s="1"/>
-      <c r="I13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1">
+        <v>7.88</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>7.88</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="1">
+        <v>12.89</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>25.78</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="1">
+        <v>7.99</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>7.99</v>
+      </c>
+      <c r="H14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E16" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{7742F5CC-94F2-40A6-A651-6CDC75B0B3F7}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{57CD3EA2-6D47-4A4F-8DFF-3E0E0D9B3D07}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{E5B1552E-2903-43BD-9BB6-4086E1052EB8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>